<commit_message>
Added example data within file
</commit_message>
<xml_diff>
--- a/GENEActiv Data Template.xlsx
+++ b/GENEActiv Data Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livekentac-my.sharepoint.com/personal/it248_kent_ac_uk/Documents/Desktop/Files/PostDoc_Kent/05. MATLAB/01. GENEActiv/Codes/GENEActiv_Data Visualisation codes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{96725E52-8D68-4D29-8924-D1CB7B336AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{202EE7BE-7A6F-4F3B-A620-138DCADB297A}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="8_{96725E52-8D68-4D29-8924-D1CB7B336AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55E03D87-70DE-4CFF-9134-ED242F8318CD}"/>
   <bookViews>
-    <workbookView xWindow="5685" yWindow="3105" windowWidth="21600" windowHeight="11175" xr2:uid="{33B35C84-3C1E-46F7-B472-D685D90BE0FF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{33B35C84-3C1E-46F7-B472-D685D90BE0FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Time stamp</t>
   </si>
@@ -72,6 +72,24 @@
   </si>
   <si>
     <t>Temperature</t>
+  </si>
+  <si>
+    <t>2025-04-23 15:55:00:000</t>
+  </si>
+  <si>
+    <t>2025-04-23 15:56:00:000</t>
+  </si>
+  <si>
+    <t>2025-04-23 15:57:00:000</t>
+  </si>
+  <si>
+    <t>2025-04-23 15:58:00:000</t>
+  </si>
+  <si>
+    <t>2025-04-23 15:59:00:000</t>
+  </si>
+  <si>
+    <t>2025-04-23 16:00:00:000</t>
   </si>
 </sst>
 </file>
@@ -443,27 +461,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{567A4335-2197-4616-8826-7BDBF3D96A11}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L34723"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -499,6 +517,234 @@
       </c>
       <c r="L1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>0.88949999999999996</v>
+      </c>
+      <c r="C2">
+        <v>0.1951</v>
+      </c>
+      <c r="D2">
+        <v>-0.1986</v>
+      </c>
+      <c r="E2">
+        <v>99</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>26.2</v>
+      </c>
+      <c r="H2">
+        <v>174.36</v>
+      </c>
+      <c r="I2">
+        <v>0.1265</v>
+      </c>
+      <c r="J2">
+        <v>0.13450000000000001</v>
+      </c>
+      <c r="K2">
+        <v>0.27639999999999998</v>
+      </c>
+      <c r="L2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>0.91159999999999997</v>
+      </c>
+      <c r="C3">
+        <v>0.15479999999999999</v>
+      </c>
+      <c r="D3">
+        <v>7.4800000000000005E-2</v>
+      </c>
+      <c r="E3">
+        <v>68</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>26</v>
+      </c>
+      <c r="H3">
+        <v>204.3</v>
+      </c>
+      <c r="I3">
+        <v>0.20039999999999999</v>
+      </c>
+      <c r="J3">
+        <v>0.2482</v>
+      </c>
+      <c r="K3">
+        <v>0.21829999999999999</v>
+      </c>
+      <c r="L3">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>0.75329999999999997</v>
+      </c>
+      <c r="C4">
+        <v>0.34410000000000002</v>
+      </c>
+      <c r="D4">
+        <v>-0.42980000000000002</v>
+      </c>
+      <c r="E4">
+        <v>125</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>25.5</v>
+      </c>
+      <c r="H4">
+        <v>206.34</v>
+      </c>
+      <c r="I4">
+        <v>0.1651</v>
+      </c>
+      <c r="J4">
+        <v>0.1026</v>
+      </c>
+      <c r="K4">
+        <v>0.249</v>
+      </c>
+      <c r="L4">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>0.75449999999999995</v>
+      </c>
+      <c r="C5">
+        <v>0.38450000000000001</v>
+      </c>
+      <c r="D5">
+        <v>-0.44950000000000001</v>
+      </c>
+      <c r="E5">
+        <v>143</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>25.5</v>
+      </c>
+      <c r="H5">
+        <v>157.93</v>
+      </c>
+      <c r="I5">
+        <v>0.1061</v>
+      </c>
+      <c r="J5">
+        <v>0.13070000000000001</v>
+      </c>
+      <c r="K5">
+        <v>0.10920000000000001</v>
+      </c>
+      <c r="L5">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>0.57469999999999999</v>
+      </c>
+      <c r="C6">
+        <v>6.9500000000000006E-2</v>
+      </c>
+      <c r="D6">
+        <v>-0.61070000000000002</v>
+      </c>
+      <c r="E6">
+        <v>103</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>25.5</v>
+      </c>
+      <c r="H6">
+        <v>191.49</v>
+      </c>
+      <c r="I6">
+        <v>0.35549999999999998</v>
+      </c>
+      <c r="J6">
+        <v>0.1734</v>
+      </c>
+      <c r="K6">
+        <v>0.3367</v>
+      </c>
+      <c r="L6">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>0.52939999999999998</v>
+      </c>
+      <c r="C7">
+        <v>0.1376</v>
+      </c>
+      <c r="D7">
+        <v>-0.3881</v>
+      </c>
+      <c r="E7">
+        <v>175</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>25.2</v>
+      </c>
+      <c r="H7">
+        <v>526.95000000000005</v>
+      </c>
+      <c r="I7">
+        <v>0.45860000000000001</v>
+      </c>
+      <c r="J7">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="K7">
+        <v>0.33879999999999999</v>
+      </c>
+      <c r="L7">
+        <v>371</v>
       </c>
     </row>
   </sheetData>

</xml_diff>